<commit_message>
Add pip to install modules in README
</commit_message>
<xml_diff>
--- a/template_frames_160_bpm_90.xlsx
+++ b/template_frames_160_bpm_90.xlsx
@@ -82,7 +82,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -130,7 +130,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -139,10 +139,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -458,7 +458,7 @@
     <col min="4" max="4" style="7" width="29.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1">
         <v>144</v>
       </c>

</xml_diff>

<commit_message>
Fix bug in motions representation
</commit_message>
<xml_diff>
--- a/template_frames_160_bpm_90.xlsx
+++ b/template_frames_160_bpm_90.xlsx
@@ -14,15 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>bpm</t>
   </si>
   <si>
-    <t>0071@000_0_0.npy</t>
-  </si>
-  <si>
-    <t>0071@002_50_0.npy</t>
+    <t>s_07_act_08_subact_01_ca_01.npy</t>
   </si>
   <si>
     <t>0071@012_60_0.npy</t>
@@ -72,7 +69,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +80,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -129,13 +132,13 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -458,7 +461,7 @@
     <col min="4" max="4" style="7" width="29.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1">
         <v>144</v>
       </c>
@@ -473,55 +476,55 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
       <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>